<commit_message>
docs: update requisitos excel
</commit_message>
<xml_diff>
--- a/Docs/Requisitos.xlsx
+++ b/Docs/Requisitos.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="129">
   <si>
     <t xml:space="preserve">CÓDIGO DO REQUISITO</t>
   </si>
@@ -154,6 +154,9 @@
     <t xml:space="preserve">Precisamos colocar os estabelecimentos em uma ordem aonde os que estão abertos fiquem primeiros e só depois os que estão fechados e sem funcionar naquele momento.</t>
   </si>
   <si>
+    <t xml:space="preserve">11-Test</t>
+  </si>
+  <si>
     <t xml:space="preserve">Script banco de dados SQL Server</t>
   </si>
   <si>
@@ -163,6 +166,9 @@
     <t xml:space="preserve">Tecnico</t>
   </si>
   <si>
+    <t xml:space="preserve">12-Test</t>
+  </si>
+  <si>
     <t xml:space="preserve">Login consumidor e estabelecimento</t>
   </si>
   <si>
@@ -172,24 +178,36 @@
     <t xml:space="preserve">Fazendo</t>
   </si>
   <si>
+    <t xml:space="preserve">13-Test</t>
+  </si>
+  <si>
     <t xml:space="preserve">Responsividade</t>
   </si>
   <si>
     <t xml:space="preserve">Precisamos que o site web seja responsivo tanto para tablet, celular e desktops</t>
   </si>
   <si>
+    <t xml:space="preserve">14-Test</t>
+  </si>
+  <si>
     <t xml:space="preserve">Dark mode</t>
   </si>
   <si>
     <t xml:space="preserve">Precisamos que dentro do site, tenhamos a possibilidade do usuário decidir o seu tema (light ou dark)</t>
   </si>
   <si>
+    <t xml:space="preserve">15-Test</t>
+  </si>
+  <si>
     <t xml:space="preserve">Preferencias </t>
   </si>
   <si>
     <t xml:space="preserve">Dado que o usuário esta logado, ele pode salvar suas prefencias de tamanhos de fonte, zoom e tema.</t>
   </si>
   <si>
+    <t xml:space="preserve">16-Test</t>
+  </si>
+  <si>
     <t xml:space="preserve">Mapa</t>
   </si>
   <si>
@@ -199,76 +217,196 @@
     <t xml:space="preserve">Desejavel</t>
   </si>
   <si>
+    <t xml:space="preserve">17-Test</t>
+  </si>
+  <si>
     <t xml:space="preserve">Suporte</t>
   </si>
   <si>
     <t xml:space="preserve">Temos que ter um meio de suporte para o consumidor ou estabelecimento se comunicar, fazer reclamações, melhorias ou outros para sabermos</t>
   </si>
   <si>
+    <t xml:space="preserve">18-Test</t>
+  </si>
+  <si>
     <t xml:space="preserve">Banco de dados Azure</t>
   </si>
   <si>
     <t xml:space="preserve">Temos que ter nosso banco de dados SQL Server hospedado na Azure para nossa aplicação acessar a mesma base de dados</t>
   </si>
   <si>
+    <t xml:space="preserve">19-Test</t>
+  </si>
+  <si>
     <t xml:space="preserve">Container Docker SQL Server</t>
   </si>
   <si>
     <t xml:space="preserve">Temos que criar uma imagem com o docker para iniciarmos o nosso banco de dados locamente sem a necessidade de usar o banco Azure</t>
   </si>
   <si>
+    <t xml:space="preserve">20-Test</t>
+  </si>
+  <si>
     <t xml:space="preserve">Configuração da identidade visual no Frontend</t>
   </si>
   <si>
     <t xml:space="preserve">Temos que criar as variaveis e defaults do projeto React no frontend, ajudará muito no desenvolvimento para facilitar e melhorar o desenvolvimento</t>
   </si>
   <si>
+    <t xml:space="preserve">21-Test</t>
+  </si>
+  <si>
     <t xml:space="preserve">Resetar senha</t>
   </si>
   <si>
     <t xml:space="preserve">Caso o usuário esqueca a senha de seu login, devemos ter uma tela para ele recuperar a senha dele</t>
   </si>
   <si>
+    <t xml:space="preserve">22-Test</t>
+  </si>
+  <si>
     <t xml:space="preserve">Envio de e-mail</t>
   </si>
   <si>
     <t xml:space="preserve">Temos que ter um serviço para envio de e-mails na plataforma</t>
   </si>
   <si>
+    <t xml:space="preserve">23-Test</t>
+  </si>
+  <si>
     <t xml:space="preserve">Cadastro de produto </t>
   </si>
   <si>
     <t xml:space="preserve">Temos que ter uma tela intuitiva e com uma boa experiencia para o usuário para o estabelecimento cadastrar as informações do seu consumível com facilidade</t>
   </si>
   <si>
+    <t xml:space="preserve">24-Test</t>
+  </si>
+  <si>
     <t xml:space="preserve">Ingredientes</t>
   </si>
   <si>
     <t xml:space="preserve">O estabelecimento na hora do cadastro do produto, deve colocar os ingredientes que foram feito aquele consumível.</t>
   </si>
   <si>
+    <t xml:space="preserve">25-Test</t>
+  </si>
+  <si>
     <t xml:space="preserve">Selo Safe Food</t>
   </si>
   <si>
     <t xml:space="preserve">Teremos a opção de na hora da criação do estabelecimento, a opção dele fazer o upload de um certificado que comprove de fato de que o estabelecimento é seguro, por sua vez será enviado um e-mail para a Safe Food validar ou não esse certificado. Esses estabelecimentos com esse “selo de segurança da Safe Food” serão mostrados com maior prioridade para o consumidor.</t>
   </si>
   <si>
+    <t xml:space="preserve">26-Test</t>
+  </si>
+  <si>
     <t xml:space="preserve">Acessebilidade</t>
   </si>
   <si>
     <t xml:space="preserve">Implementar tecnicas de acessibilidade para o projeto (leitura de texto, inverter as cores, zoom, aumento de fonte, dark mode, html semantico)</t>
   </si>
   <si>
+    <t xml:space="preserve">27-Test</t>
+  </si>
+  <si>
     <t xml:space="preserve">Cache dos principais consumiveis</t>
   </si>
   <si>
     <t xml:space="preserve">Temos que implementar uma camada de cache com Redis no Backend para melhorar a velocidade da requisição para o usuário, não tenha de esperar muito</t>
   </si>
   <si>
+    <t xml:space="preserve">28-Test</t>
+  </si>
+  <si>
     <t xml:space="preserve">Deploy Conitinuo Azure</t>
   </si>
   <si>
     <t xml:space="preserve">Ao chegar um commit na branch main do frontend, deve acionar a ação e fazer o deploy automaticamente no sistema azure, para que em poucos instantes possamos acessar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">29-Test</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gerenciamento dos consumiveis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Deve ser possível de alterar descrições, titulos e outros dados dos consumiveís, ou mesmo decidir apaga-los ou desativa-los.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">30-Test</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cadastro do estabelecimento</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Para que seja possível o cadastro de produto, devemos a priori ter o cadastro de estabelecimento dentro da plataoforma</t>
+  </si>
+  <si>
+    <t xml:space="preserve">31-Test</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Placeholder de textos da plataforma</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Os textos da plataforma devem ter um contexto, por exemplo a tela de sobre e de termos de uso devem estar completas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">32-Test</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Placeholder da pesquisa de consumiveis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Deve aparecer sugestões de textos e itens quando formos pesquisar dentro da barra de pesquisa da plataforma</t>
+  </si>
+  <si>
+    <t xml:space="preserve">33-Test</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Visitar perfil estabelecimento e consumidores</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Para mais detalhes de um estabelecimento ou mesmo de um consumidor, devemos poder acessar a página de perfil dele vendo seus detalhes, como favoritos e comentários ou pra estabelecimento seus produtos diretamente</t>
+  </si>
+  <si>
+    <t xml:space="preserve">34-Test</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dashboard estabelecimento</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Um dashboard simples mostrando o Rate de seus produtos e os comentários de tal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">35-Test</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CDN páginas estáticas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Para uma melhor experiencia do usuário, podemos utilizar uma ferramenta de CDN (Content Delivery Network) que ajudará na hospedagem de conteudo estatico do site, deixando-o mais fluido</t>
+  </si>
+  <si>
+    <t xml:space="preserve">36-Test</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Static incremental Generation Next</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Junto a linha de CDN, podemos usar o Next para fazer o ISR, para que seja mais rapido e tenhamos um cache em produção das páginas estáticas que não mudam</t>
+  </si>
+  <si>
+    <t xml:space="preserve">37-Test</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Local armazenamento de imagens</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Precisamos armazenar as imagens em algum lugar para que assim façamos o upload das próprias no local adequado, e quando precisamos podemos acessa-las via URL (Ex: Amazon S3)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">38-Test</t>
   </si>
 </sst>
 </file>
@@ -478,13 +616,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="A1:H38"/>
+  <dimension ref="A1:H54"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="40" zoomScaleNormal="40" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E35" activeCellId="0" sqref="E35"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="32.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="69"/>
@@ -522,7 +660,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="28.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="n">
         <v>1</v>
       </c>
@@ -548,7 +686,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="28.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="n">
         <v>2</v>
       </c>
@@ -574,7 +712,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="28.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="n">
         <v>3</v>
       </c>
@@ -600,7 +738,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="28.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="5" t="n">
         <v>4</v>
       </c>
@@ -626,7 +764,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="28.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="5" t="n">
         <v>5</v>
       </c>
@@ -652,7 +790,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="28.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="5" t="n">
         <v>6</v>
       </c>
@@ -678,7 +816,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="44" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="42.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="5" t="n">
         <v>7</v>
       </c>
@@ -704,7 +842,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="5" t="n">
         <v>8</v>
       </c>
@@ -730,7 +868,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="27.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="5" t="n">
         <v>9</v>
       </c>
@@ -804,7 +942,9 @@
       <c r="G12" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="H12" s="5"/>
+      <c r="H12" s="5" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="5" t="n">
@@ -814,21 +954,23 @@
         <v>12</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E13" s="6" t="s">
         <v>10</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="G13" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="H13" s="5"/>
+      <c r="H13" s="5" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="5" t="n">
@@ -838,10 +980,10 @@
         <v>13</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="E14" s="6" t="s">
         <v>10</v>
@@ -850,9 +992,11 @@
         <v>11</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="H14" s="5"/>
+        <v>51</v>
+      </c>
+      <c r="H14" s="5" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="5" t="n">
@@ -862,21 +1006,23 @@
         <v>14</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="E15" s="6" t="s">
         <v>10</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="G15" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="H15" s="5"/>
+      <c r="H15" s="5" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="5" t="n">
@@ -886,21 +1032,23 @@
         <v>15</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E16" s="6" t="s">
         <v>16</v>
       </c>
       <c r="F16" s="6" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="G16" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="H16" s="5"/>
+      <c r="H16" s="5" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="5" t="n">
@@ -910,33 +1058,39 @@
         <v>16</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="E17" s="6" t="s">
         <v>16</v>
       </c>
       <c r="F17" s="6" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="G17" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="H17" s="5"/>
+      <c r="H17" s="5" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="5"/>
-      <c r="B18" s="5"/>
+      <c r="A18" s="5" t="n">
+        <v>17</v>
+      </c>
+      <c r="B18" s="5" t="n">
+        <v>17</v>
+      </c>
       <c r="C18" s="5" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="F18" s="6" t="s">
         <v>11</v>
@@ -944,16 +1098,22 @@
       <c r="G18" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="H18" s="5"/>
+      <c r="H18" s="5" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="5"/>
-      <c r="B19" s="5"/>
+      <c r="A19" s="5" t="n">
+        <v>18</v>
+      </c>
+      <c r="B19" s="5" t="n">
+        <v>18</v>
+      </c>
       <c r="C19" s="5" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="E19" s="6" t="s">
         <v>16</v>
@@ -964,76 +1124,100 @@
       <c r="G19" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="H19" s="5"/>
+      <c r="H19" s="5" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="5"/>
-      <c r="B20" s="5"/>
+      <c r="A20" s="5" t="n">
+        <v>19</v>
+      </c>
+      <c r="B20" s="5" t="n">
+        <v>19</v>
+      </c>
       <c r="C20" s="5" t="s">
-        <v>61</v>
+        <v>69</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>62</v>
+        <v>70</v>
       </c>
       <c r="E20" s="6" t="s">
         <v>10</v>
       </c>
       <c r="F20" s="6" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="G20" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="H20" s="5"/>
+      <c r="H20" s="5" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="5"/>
-      <c r="B21" s="5"/>
+      <c r="A21" s="5" t="n">
+        <v>20</v>
+      </c>
+      <c r="B21" s="5" t="n">
+        <v>20</v>
+      </c>
       <c r="C21" s="5" t="s">
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>64</v>
+        <v>73</v>
       </c>
       <c r="E21" s="6" t="s">
         <v>16</v>
       </c>
       <c r="F21" s="6" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="G21" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="H21" s="5"/>
+      <c r="H21" s="5" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="5"/>
-      <c r="B22" s="5"/>
+      <c r="A22" s="5" t="n">
+        <v>21</v>
+      </c>
+      <c r="B22" s="5" t="n">
+        <v>21</v>
+      </c>
       <c r="C22" s="5" t="s">
-        <v>65</v>
+        <v>75</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>66</v>
+        <v>76</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="F22" s="6" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="G22" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="H22" s="5"/>
+      <c r="H22" s="5" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="5"/>
-      <c r="B23" s="5"/>
+      <c r="A23" s="5" t="n">
+        <v>22</v>
+      </c>
+      <c r="B23" s="5" t="n">
+        <v>22</v>
+      </c>
       <c r="C23" s="5" t="s">
-        <v>67</v>
+        <v>78</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>68</v>
+        <v>79</v>
       </c>
       <c r="E23" s="6" t="s">
         <v>16</v>
@@ -1044,36 +1228,48 @@
       <c r="G23" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="H23" s="5"/>
+      <c r="H23" s="5" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="5"/>
-      <c r="B24" s="5"/>
+      <c r="A24" s="5" t="n">
+        <v>23</v>
+      </c>
+      <c r="B24" s="5" t="n">
+        <v>23</v>
+      </c>
       <c r="C24" s="5" t="s">
-        <v>69</v>
+        <v>81</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>70</v>
+        <v>82</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="F24" s="6" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="G24" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="H24" s="5"/>
+      <c r="H24" s="5" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="25" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="5"/>
-      <c r="B25" s="5"/>
+      <c r="A25" s="5" t="n">
+        <v>24</v>
+      </c>
+      <c r="B25" s="5" t="n">
+        <v>24</v>
+      </c>
       <c r="C25" s="5" t="s">
-        <v>71</v>
+        <v>84</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>72</v>
+        <v>85</v>
       </c>
       <c r="E25" s="6" t="s">
         <v>10</v>
@@ -1084,16 +1280,22 @@
       <c r="G25" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="H25" s="5"/>
+      <c r="H25" s="5" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="26" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="5"/>
-      <c r="B26" s="5"/>
+      <c r="A26" s="5" t="n">
+        <v>25</v>
+      </c>
+      <c r="B26" s="5" t="n">
+        <v>25</v>
+      </c>
       <c r="C26" s="5" t="s">
-        <v>73</v>
+        <v>87</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>74</v>
+        <v>88</v>
       </c>
       <c r="E26" s="6" t="s">
         <v>16</v>
@@ -1104,19 +1306,25 @@
       <c r="G26" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="H26" s="5"/>
+      <c r="H26" s="5" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="27" customFormat="false" ht="58.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="5"/>
-      <c r="B27" s="5"/>
+      <c r="A27" s="5" t="n">
+        <v>26</v>
+      </c>
+      <c r="B27" s="5" t="n">
+        <v>26</v>
+      </c>
       <c r="C27" s="5" t="s">
-        <v>75</v>
+        <v>90</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>76</v>
+        <v>91</v>
       </c>
       <c r="E27" s="6" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="F27" s="6" t="s">
         <v>11</v>
@@ -1124,16 +1332,22 @@
       <c r="G27" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="H27" s="5"/>
+      <c r="H27" s="5" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="28" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="5"/>
-      <c r="B28" s="5"/>
+      <c r="A28" s="5" t="n">
+        <v>27</v>
+      </c>
+      <c r="B28" s="5" t="n">
+        <v>27</v>
+      </c>
       <c r="C28" s="5" t="s">
-        <v>77</v>
+        <v>93</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>78</v>
+        <v>94</v>
       </c>
       <c r="E28" s="6" t="s">
         <v>16</v>
@@ -1144,127 +1358,445 @@
       <c r="G28" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="H28" s="5"/>
+      <c r="H28" s="5" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="29" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="5"/>
-      <c r="B29" s="5"/>
+      <c r="A29" s="5" t="n">
+        <v>28</v>
+      </c>
+      <c r="B29" s="5" t="n">
+        <v>28</v>
+      </c>
       <c r="C29" s="5" t="s">
-        <v>79</v>
+        <v>96</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>80</v>
+        <v>97</v>
       </c>
       <c r="E29" s="6" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="F29" s="6" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="G29" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="H29" s="5"/>
+      <c r="H29" s="5" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="30" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="5"/>
-      <c r="B30" s="5"/>
+      <c r="A30" s="5" t="n">
+        <v>29</v>
+      </c>
+      <c r="B30" s="5" t="n">
+        <v>29</v>
+      </c>
       <c r="C30" s="5" t="s">
-        <v>81</v>
+        <v>99</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>82</v>
+        <v>100</v>
       </c>
       <c r="E30" s="6" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="F30" s="6" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="G30" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="H30" s="5"/>
-    </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="5"/>
-      <c r="B31" s="5"/>
-      <c r="C31" s="5"/>
-      <c r="D31" s="5"/>
-      <c r="E31" s="6"/>
-      <c r="F31" s="6"/>
-      <c r="G31" s="5"/>
-      <c r="H31" s="5"/>
-    </row>
-    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="5"/>
-      <c r="B32" s="5"/>
-      <c r="C32" s="5"/>
-      <c r="D32" s="5"/>
-      <c r="E32" s="6"/>
-      <c r="F32" s="6"/>
-      <c r="G32" s="5"/>
-      <c r="H32" s="5"/>
-    </row>
-    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="5"/>
-      <c r="B33" s="5"/>
-      <c r="C33" s="5"/>
-      <c r="D33" s="5"/>
-      <c r="E33" s="6"/>
-      <c r="F33" s="6"/>
-      <c r="G33" s="5"/>
-      <c r="H33" s="5"/>
-    </row>
-    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="5"/>
-      <c r="B34" s="5"/>
-      <c r="C34" s="5"/>
-      <c r="D34" s="5"/>
-      <c r="E34" s="6"/>
-      <c r="F34" s="6"/>
-      <c r="G34" s="5"/>
-      <c r="H34" s="5"/>
-    </row>
-    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="5"/>
-      <c r="B35" s="5"/>
-      <c r="C35" s="5"/>
-      <c r="D35" s="5"/>
-      <c r="E35" s="6"/>
-      <c r="F35" s="6"/>
-      <c r="G35" s="5"/>
-      <c r="H35" s="5"/>
-    </row>
-    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="5"/>
-      <c r="B36" s="5"/>
-      <c r="C36" s="5"/>
-      <c r="D36" s="5"/>
-      <c r="E36" s="6"/>
-      <c r="F36" s="6"/>
-      <c r="G36" s="5"/>
-      <c r="H36" s="5"/>
-    </row>
-    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="5"/>
-      <c r="B37" s="5"/>
-      <c r="C37" s="5"/>
-      <c r="D37" s="5"/>
-      <c r="E37" s="6"/>
-      <c r="F37" s="6"/>
-      <c r="G37" s="5"/>
-      <c r="H37" s="5"/>
-    </row>
-    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="5"/>
-      <c r="B38" s="5"/>
-      <c r="C38" s="5"/>
-      <c r="D38" s="5"/>
-      <c r="E38" s="6"/>
-      <c r="F38" s="6"/>
-      <c r="G38" s="5"/>
-      <c r="H38" s="5"/>
+      <c r="H30" s="5" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="5" t="n">
+        <v>30</v>
+      </c>
+      <c r="B31" s="5" t="n">
+        <v>30</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="D31" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="E31" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F31" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G31" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H31" s="5" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="5" t="n">
+        <v>31</v>
+      </c>
+      <c r="B32" s="5" t="n">
+        <v>31</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="E32" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F32" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G32" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H32" s="5" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="5" t="n">
+        <v>32</v>
+      </c>
+      <c r="B33" s="5" t="n">
+        <v>32</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="E33" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F33" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="G33" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H33" s="5" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="15.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="B34" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="E34" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="F34" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G34" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H34" s="5" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="43.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="5" t="n">
+        <v>34</v>
+      </c>
+      <c r="B35" s="5" t="n">
+        <v>34</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="D35" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="E35" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="F35" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G35" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H35" s="5" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="15.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="5" t="n">
+        <v>35</v>
+      </c>
+      <c r="B36" s="5" t="n">
+        <v>35</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="D36" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="E36" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="F36" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G36" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H36" s="5" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="5" t="n">
+        <v>36</v>
+      </c>
+      <c r="B37" s="5" t="n">
+        <v>36</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="D37" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="E37" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="F37" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="G37" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H37" s="5" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="5" t="n">
+        <v>37</v>
+      </c>
+      <c r="B38" s="5" t="n">
+        <v>37</v>
+      </c>
+      <c r="C38" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="D38" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="E38" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="F38" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="G38" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H38" s="5" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="5" t="n">
+        <v>38</v>
+      </c>
+      <c r="B39" s="5" t="n">
+        <v>38</v>
+      </c>
+      <c r="C39" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="D39" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="E39" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F39" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="G39" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H39" s="5" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="5"/>
+      <c r="B40" s="5"/>
+      <c r="C40" s="5"/>
+      <c r="D40" s="5"/>
+      <c r="E40" s="6"/>
+      <c r="F40" s="6"/>
+      <c r="G40" s="5"/>
+      <c r="H40" s="5"/>
+    </row>
+    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="5"/>
+      <c r="B41" s="5"/>
+      <c r="C41" s="5"/>
+      <c r="D41" s="5"/>
+      <c r="E41" s="6"/>
+      <c r="F41" s="6"/>
+      <c r="G41" s="5"/>
+      <c r="H41" s="5"/>
+    </row>
+    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="5"/>
+      <c r="B42" s="5"/>
+      <c r="C42" s="5"/>
+      <c r="D42" s="5"/>
+      <c r="E42" s="6"/>
+      <c r="F42" s="6"/>
+      <c r="G42" s="5"/>
+      <c r="H42" s="5"/>
+    </row>
+    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="5"/>
+      <c r="B43" s="5"/>
+      <c r="C43" s="5"/>
+      <c r="D43" s="5"/>
+      <c r="E43" s="6"/>
+      <c r="F43" s="6"/>
+      <c r="G43" s="5"/>
+      <c r="H43" s="5"/>
+    </row>
+    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="5"/>
+      <c r="B44" s="5"/>
+      <c r="C44" s="5"/>
+      <c r="D44" s="5"/>
+      <c r="E44" s="6"/>
+      <c r="F44" s="6"/>
+      <c r="G44" s="5"/>
+      <c r="H44" s="5"/>
+    </row>
+    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="5"/>
+      <c r="B45" s="5"/>
+      <c r="C45" s="5"/>
+      <c r="D45" s="5"/>
+      <c r="E45" s="6"/>
+      <c r="F45" s="6"/>
+      <c r="G45" s="5"/>
+      <c r="H45" s="5"/>
+    </row>
+    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="5"/>
+      <c r="B46" s="5"/>
+      <c r="C46" s="5"/>
+      <c r="D46" s="5"/>
+      <c r="E46" s="6"/>
+      <c r="F46" s="6"/>
+      <c r="G46" s="5"/>
+      <c r="H46" s="5"/>
+    </row>
+    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="5"/>
+      <c r="B47" s="5"/>
+      <c r="C47" s="5"/>
+      <c r="D47" s="5"/>
+      <c r="E47" s="6"/>
+      <c r="F47" s="6"/>
+      <c r="G47" s="5"/>
+      <c r="H47" s="5"/>
+    </row>
+    <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="5"/>
+      <c r="B48" s="5"/>
+      <c r="C48" s="5"/>
+      <c r="D48" s="5"/>
+      <c r="E48" s="6"/>
+      <c r="F48" s="6"/>
+      <c r="G48" s="5"/>
+      <c r="H48" s="5"/>
+    </row>
+    <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="5"/>
+      <c r="B49" s="5"/>
+      <c r="C49" s="5"/>
+      <c r="D49" s="5"/>
+      <c r="E49" s="6"/>
+      <c r="F49" s="6"/>
+      <c r="G49" s="5"/>
+      <c r="H49" s="5"/>
+    </row>
+    <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="5"/>
+      <c r="B50" s="5"/>
+      <c r="C50" s="5"/>
+      <c r="D50" s="5"/>
+      <c r="E50" s="6"/>
+      <c r="F50" s="6"/>
+      <c r="G50" s="5"/>
+      <c r="H50" s="5"/>
+    </row>
+    <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="5"/>
+      <c r="B51" s="5"/>
+      <c r="C51" s="5"/>
+      <c r="D51" s="5"/>
+      <c r="E51" s="6"/>
+      <c r="F51" s="6"/>
+      <c r="G51" s="5"/>
+      <c r="H51" s="5"/>
+    </row>
+    <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="5"/>
+      <c r="B52" s="5"/>
+      <c r="C52" s="5"/>
+      <c r="D52" s="5"/>
+      <c r="E52" s="6"/>
+      <c r="F52" s="6"/>
+      <c r="G52" s="5"/>
+      <c r="H52" s="5"/>
+    </row>
+    <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="5"/>
+      <c r="B53" s="5"/>
+      <c r="C53" s="5"/>
+      <c r="D53" s="5"/>
+      <c r="E53" s="6"/>
+      <c r="F53" s="6"/>
+      <c r="G53" s="5"/>
+      <c r="H53" s="5"/>
+    </row>
+    <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="5"/>
+      <c r="B54" s="5"/>
+      <c r="C54" s="5"/>
+      <c r="D54" s="5"/>
+      <c r="E54" s="6"/>
+      <c r="F54" s="6"/>
+      <c r="G54" s="5"/>
+      <c r="H54" s="5"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>